<commit_message>
update bugs in MMFAD9A
</commit_message>
<xml_diff>
--- a/scoring/tests/MMFAD/MMFAD93_test_1.xlsx
+++ b/scoring/tests/MMFAD/MMFAD93_test_1.xlsx
@@ -460,7 +460,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -500,7 +500,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -520,7 +520,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -560,7 +560,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -580,7 +580,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -600,7 +600,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -610,7 +610,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -620,7 +620,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -660,7 +660,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -680,7 +680,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -720,7 +720,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -730,7 +730,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -740,7 +740,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -750,7 +750,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -770,7 +770,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -780,7 +780,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -790,7 +790,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -800,7 +800,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -810,7 +810,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -840,7 +840,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -850,7 +850,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -880,7 +880,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -890,7 +890,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -910,7 +910,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -920,7 +920,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -930,7 +930,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -940,7 +940,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -960,7 +960,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>